<commit_message>
feat: add new row for brands
</commit_message>
<xml_diff>
--- a/public/DataBrands/BrandImport.xlsx
+++ b/public/DataBrands/BrandImport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwiie\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B381635-C4CA-4618-A5F8-94E39D736AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F39EACE-84FB-4F87-B1FE-C2697A1B4E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{DA9A031A-BBD2-45D8-ACF5-8D4E235C4FBC}"/>
   </bookViews>
@@ -34,15 +34,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Wawi</t>
   </si>
   <si>
-    <t>Dwi</t>
+    <t>owner</t>
   </si>
   <si>
-    <t>test</t>
+    <t>founded_date</t>
+  </si>
+  <si>
+    <t>brand_name</t>
+  </si>
+  <si>
+    <t>Keebs.id</t>
   </si>
 </sst>
 </file>
@@ -78,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,48 +401,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF61177A-0685-43E5-8C0F-E5E760058051}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45517</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>